<commit_message>
Add best.py model trained on custom dataset
</commit_message>
<xml_diff>
--- a/test.dav.xlsx
+++ b/test.dav.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F7"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,25 +429,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>motorcycle</t>
+          <t>sitp</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>truck</t>
+          <t>scooter</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>motorbike</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>car</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>bicycle</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2-axis</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>bus</t>
         </is>
@@ -463,15 +473,21 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -482,19 +498,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="E4" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F4" t="n">
         <v>5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -507,16 +529,22 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
+      <c r="H5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -529,15 +557,21 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -565,6 +599,14 @@
       </c>
       <c r="F7">
         <f>SUM(F3:F6)</f>
+        <v/>
+      </c>
+      <c r="G7">
+        <f>SUM(G3:G6)</f>
+        <v/>
+      </c>
+      <c r="H7">
+        <f>SUM(H3:H6)</f>
         <v/>
       </c>
     </row>

</xml_diff>